<commit_message>
ticker from market name
</commit_message>
<xml_diff>
--- a/data/couple_coin_list.xlsx
+++ b/data/couple_coin_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>선두코인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>KRW-XRP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>가격대</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -50,10 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>KRW-XLM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아슨스리 커플링</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,19 +54,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>KRW-QKC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KRW-IOST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>중국코인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>20~50원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리플</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스텔라루멘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿼크체인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이오에스티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리스크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오미세고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000~3000원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격대 커플링</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,14 +425,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="5" max="5" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -427,41 +449,58 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coupling lists are added
</commit_message>
<xml_diff>
--- a/data/couple_coin_list.xlsx
+++ b/data/couple_coin_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>선두코인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,126 @@
   </si>
   <si>
     <t>가격대 커플링</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리퍼리움</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엠블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스톰엑스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이오에스티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골렘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아더</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아르고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스팀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이브</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메탈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웨이브</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코박토큰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파쿼크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플로우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>던프로토콜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>샌드박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디센트럴랜드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세럼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퀀텀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네오</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비트토렌트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메디블록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메타디움</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -503,8 +623,163 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>